<commit_message>
Deploying to gh-pages from  @ eb0cd89476d61b54e21552d71f2b56c11fef7e81 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_3-1-1.xlsx
+++ b/assets/excel/2022_3-1-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94960CAC-CC64-464C-9D03-AD19315DABCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{696A789E-E07E-42BB-90F8-1F56DDB52809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{A3E2701A-2D3A-44CD-B552-8314618F32E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{38F2E506-5172-4690-BBA6-32D35DD66F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <t>1) Anteil der Kinder in öffentlich geförderter Kindertagespflege, die nicht zusätzlich eine Einrichtung der Kindertagesbetreuung oder eine Ganztagsschule besuchen, sowie der Kinder in Kindertageseinrichtungen an allen Kindern in der gleichen Altersgruppe. Da in der Statistik zur Kindertagesbetreuung die Anzahl der betreuten Kinder im jeweiligen Kreis ermittelt wird und keine Zuordnung der Kinder zu ihrem Wohnort erfolgt, kann die Betreuungsquote in einzelnen Kreisen oder evtl. auch in einem Bundesland in Ausnahmefällen über 100 % liegen.</t>
   </si>
   <si>
-    <t>Quellen: Statistische Ämter des Bundes und der Länder, Kindertagesbetreuung regional; Kinder- und Jugendhilfestatistik / Statistisches Bundesamt; Kinder- und Jugendhilfestatistik, Mikrozensus, Bevölkerungsstatistik</t>
+    <t>Quellen: Statistische Ämter des Bundes und der Länder, Kindertagesbetreuung regional 2018; Kinder- und Jugendhilfestatistik / Statistisches Bundesamt; Kinder- und Jugendhilfestatistik, Mikrozensus, Bevölkerungsstatistik</t>
   </si>
   <si>
     <t>Niedersächsisches Ministerium für Soziales, Gesundheit und Gleichstellung (Hrsg.),</t>
@@ -101,11 +101,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="5">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="##\ ##\ ##\ ###"/>
+    <numFmt numFmtId="170" formatCode="##\ ##"/>
+    <numFmt numFmtId="171" formatCode="##\ ##\ #"/>
+    <numFmt numFmtId="172" formatCode="##\ ##\ ##"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +118,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="NDSFrutiger 55 Roman"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -123,13 +140,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="NDSFrutiger 55 Roman"/>
-    </font>
-    <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="6"/>
@@ -141,17 +154,22 @@
       <name val="NDSFrutiger 45 Light"/>
     </font>
     <font>
-      <u/>
+      <sz val="9"/>
+      <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 45 Light"/>
     </font>
     <font>
       <u/>
       <sz val="6"/>
-      <color theme="10"/>
+      <color indexed="12"/>
       <name val="NDSFrutiger 45 Light"/>
     </font>
   </fonts>
@@ -172,30 +190,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -218,6 +212,15 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -228,14 +231,14 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -261,6 +264,30 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -280,109 +307,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
+    <cellStyle name="4" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="5" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="6" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="9" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Tabellenformat 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -690,912 +755,956 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397E1C7A-5769-4F9D-AA28-C632693502FD}">
-  <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:J46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57A5C80-7F38-4918-8840-53E3EE7287B6}">
+  <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="9" width="11" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="8" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="10" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="16"/>
+      <c r="J8" s="24"/>
+    </row>
+    <row r="9" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
       <c r="C9" s="17"/>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="18">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="25">
         <v>1</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="5">
         <v>3</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="5">
         <v>4</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="5">
         <v>5</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="5">
         <v>6</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="5">
         <v>7</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="6">
         <v>8</v>
       </c>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="21" t="s">
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="26">
         <v>2009</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="27">
         <v>11.9</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="27">
         <v>88.1</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="27">
         <v>6.1</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="27">
         <v>75.599999999999994</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="27">
         <v>14.4</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="27">
         <v>93.2</v>
       </c>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="21" t="s">
+      <c r="J11" s="28"/>
+    </row>
+    <row r="12" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="26">
         <v>2009</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="27">
         <v>20.2</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="27">
         <v>91.6</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="27">
         <v>10.5</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="27">
         <v>83.6</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="27">
         <v>24.8</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="27">
         <v>95.6</v>
       </c>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="21" t="s">
+      <c r="J12" s="28"/>
+    </row>
+    <row r="13" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="26">
         <v>2010</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="27">
         <v>15.8</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="27">
         <v>89.5</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="27">
         <v>8</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="27">
         <v>79.3</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="27">
         <v>18.8</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="27">
         <v>92.9</v>
       </c>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="21" t="s">
+      <c r="J13" s="28"/>
+    </row>
+    <row r="14" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="26">
         <v>2010</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="27">
         <v>23</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="27">
         <v>92.2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="27">
         <v>12.2</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="27">
         <v>85.7</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="27">
         <v>27.7</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="27">
         <v>94.9</v>
       </c>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="21" t="s">
+      <c r="J14" s="28"/>
+    </row>
+    <row r="15" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="26">
         <v>2011</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="27">
         <v>18.600000000000001</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="27">
         <v>91.6</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="27">
         <v>9.2360000000000007</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="27">
         <v>82.67</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="27">
         <v>22.46</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="27">
         <v>94.668999999999997</v>
       </c>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="21" t="s">
+      <c r="J15" s="28"/>
+    </row>
+    <row r="16" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="26">
         <v>2011</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="27">
         <v>25.2</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="27">
         <v>93</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="27">
         <v>13.965999999999999</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="27">
         <v>84.924000000000007</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="27">
         <v>30.058</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="27">
         <v>96.557000000000002</v>
       </c>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="21" t="s">
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="26">
         <v>2012</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="27">
         <v>22.1</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="27">
         <v>92.6</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="29">
         <v>12</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="29">
         <v>79</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="29">
         <v>26</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="29">
         <v>98</v>
       </c>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="21" t="s">
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="26">
         <v>2012</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="27">
         <v>27.6</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="27">
         <v>93.4</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="29">
         <v>16</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="29">
         <v>87</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="29">
         <v>33</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="29">
         <v>96</v>
       </c>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="21" t="s">
+      <c r="J18" s="28"/>
+    </row>
+    <row r="19" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="26">
         <v>2013</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="27">
         <v>24.4</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="27">
         <v>93.6</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="29">
         <v>13</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="29">
         <v>74</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="29">
         <v>29</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="29">
         <v>102</v>
       </c>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="21" t="s">
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="26">
         <v>2013</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="27">
         <v>29.3</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="27">
         <v>93.6</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="29">
         <v>17</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="29">
         <v>85</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="29">
         <v>35</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="29">
         <v>98</v>
       </c>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="21" t="s">
+      <c r="J20" s="28"/>
+    </row>
+    <row r="21" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="26">
         <v>2014</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="27">
         <v>27.9</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="27">
         <v>93.7</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="29">
         <v>15</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="29">
         <v>72</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="29">
         <v>33</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="29">
         <v>103</v>
       </c>
-      <c r="J21" s="23"/>
-    </row>
-    <row r="22" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="21" t="s">
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="26">
         <v>2014</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="27">
         <v>32.299999999999997</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="27">
         <v>93.6</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="29">
         <v>20</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="29">
         <v>85</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="29">
         <v>38</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="29">
         <v>98</v>
       </c>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="21" t="s">
+      <c r="J22" s="28"/>
+    </row>
+    <row r="23" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="26">
         <v>2015</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="27">
         <v>28.3</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="27">
         <v>94.8</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="29">
         <v>15</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="29">
         <v>77</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="29">
         <v>34</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="30">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="21" t="s">
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="26">
         <v>2015</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="27">
         <v>32.9</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="27">
         <v>94.9</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="29">
         <v>22</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="29">
         <v>90</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="29">
         <v>38</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="30">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="21" t="s">
+      <c r="J24" s="20"/>
+    </row>
+    <row r="25" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="26">
         <v>2016</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="31">
         <v>28.4</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="31">
         <v>93.2</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="29">
         <v>15</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="29">
         <v>78</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="29">
         <v>34</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="29">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="21" t="s">
+      <c r="J25" s="20"/>
+    </row>
+    <row r="26" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="26">
         <v>2016</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="27">
         <v>32.700000000000003</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="27">
         <v>93.6</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="29">
         <v>21</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="29">
         <v>88</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="29">
         <v>38</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="29">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="21" t="s">
+      <c r="J26" s="20"/>
+    </row>
+    <row r="27" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="26">
         <v>2017</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="31">
         <v>29.6</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="31">
         <v>93.2</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="29">
         <v>15</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="29">
         <v>71</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="29">
         <v>37</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="31">
         <v>104</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="21" t="s">
+      <c r="J27" s="20"/>
+    </row>
+    <row r="28" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="26">
         <v>2017</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="27">
         <v>33.1</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="27">
         <v>93.4</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="29">
         <v>20</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="29">
         <v>84</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="29">
         <v>40</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="30">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="21" t="s">
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="26">
         <v>2018</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="27">
         <v>30.9</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="27">
         <v>92.8</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="31">
         <v>15</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="31">
         <v>73</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="31">
         <v>39</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="31">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="21" t="s">
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="26">
         <v>2018</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="27">
         <v>33.6</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="27">
         <v>93</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="29">
         <v>20</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="29">
         <v>82</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="29">
         <v>60</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="30">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="21" t="s">
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="26">
         <v>2019</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="27">
         <v>32.1</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="27">
         <v>92.7</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="29">
         <v>16</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="29">
         <v>78</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="29">
         <v>41</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="29">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="21" t="s">
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="26">
         <v>2019</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="27">
         <v>34.299999999999997</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="27">
         <v>93</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="29">
         <v>21</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="29">
         <v>81</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="29">
         <v>42</v>
       </c>
-      <c r="I32" s="25">
+      <c r="I32" s="29">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="21" t="s">
+      <c r="J32" s="20"/>
+    </row>
+    <row r="33" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="20">
         <v>2020</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="27">
         <v>32.9</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="27">
         <v>92.2</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="29">
         <v>17</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="29">
         <v>75</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="29">
         <v>42</v>
       </c>
-      <c r="I33" s="25">
+      <c r="I33" s="29">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="21" t="s">
+      <c r="J33" s="20"/>
+    </row>
+    <row r="34" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="20">
         <v>2020</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="27">
         <v>35</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="27">
         <v>92.5</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="29">
         <v>21</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="29">
         <v>81</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="29">
         <v>43</v>
       </c>
-      <c r="I34" s="25">
+      <c r="I34" s="29">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="21" t="s">
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="2:10" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="20">
         <v>2021</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="29">
         <v>31.9</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="29">
         <v>91.6</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="2:10" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="20">
+        <v>2021</v>
+      </c>
+      <c r="D36" s="29">
+        <v>34.4</v>
+      </c>
+      <c r="E36" s="29">
+        <v>91.9</v>
+      </c>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="26"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="24"/>
+    </row>
+    <row r="38" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="36"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="24"/>
+    </row>
+    <row r="39" spans="2:10" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="2:10" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="25">
-        <v>75</v>
-      </c>
-      <c r="H35" s="25">
-        <v>38</v>
-      </c>
-      <c r="I35" s="25">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="24">
-        <v>2021</v>
-      </c>
-      <c r="D36" s="25">
-        <v>34.4</v>
-      </c>
-      <c r="E36" s="25">
-        <v>91.9</v>
-      </c>
-      <c r="F36" s="25">
-        <v>21</v>
-      </c>
-      <c r="G36" s="25">
-        <v>81</v>
-      </c>
-      <c r="H36" s="25">
-        <v>43</v>
-      </c>
-      <c r="I36" s="25">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B37" s="21"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B38" s="31"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="2:10" s="24" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-    </row>
-    <row r="40" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-    </row>
-    <row r="42" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="33" t="s">
+    </row>
+    <row r="45" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="34" t="s">
+    <row r="46" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="23" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="47" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B41:I41"/>
     <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B41:I41"/>
     <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="C6:C9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B46" r:id="rId1" xr:uid="{BCD2D9F4-B2E7-4CF8-9464-F77ABB4C38AE}"/>
+    <hyperlink ref="B46" r:id="rId1" xr:uid="{270811AE-01D9-4210-90E4-CD88FFE2C23C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 2090cc02491eb4d2f8b813347a8adc60856edd87 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_3-1-1.xlsx
+++ b/assets/excel/2022_3-1-1.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{696A789E-E07E-42BB-90F8-1F56DDB52809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974AA6E-C514-41A6-8D3F-7E6A706B4F49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{38F2E506-5172-4690-BBA6-32D35DD66F9E}"/>
   </bookViews>
@@ -103,11 +103,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="##\ ##\ ##\ ###"/>
-    <numFmt numFmtId="170" formatCode="##\ ##"/>
-    <numFmt numFmtId="171" formatCode="##\ ##\ #"/>
-    <numFmt numFmtId="172" formatCode="##\ ##\ ##"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="##\ ##\ ##\ ###"/>
+    <numFmt numFmtId="166" formatCode="##\ ##"/>
+    <numFmt numFmtId="167" formatCode="##\ ##\ #"/>
+    <numFmt numFmtId="168" formatCode="##\ ##\ ##"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -311,16 +311,16 @@
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -345,6 +345,63 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -368,63 +425,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -756,6 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57A5C80-7F38-4918-8840-53E3EE7287B6}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:J47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
@@ -826,43 +827,43 @@
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="13" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="32"/>
+      <c r="H7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="16"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="30"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
@@ -881,23 +882,23 @@
       <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="13" t="s">
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="31"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="24"/>
-    </row>
-    <row r="10" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25">
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -921,775 +922,775 @@
       <c r="I10" s="6">
         <v>8</v>
       </c>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="17">
         <v>2009</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="18">
         <v>11.9</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="18">
         <v>88.1</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="18">
         <v>6.1</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="18">
         <v>75.599999999999994</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="18">
         <v>14.4</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="18">
         <v>93.2</v>
       </c>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="17">
         <v>2009</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="18">
         <v>20.2</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="18">
         <v>91.6</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="18">
         <v>10.5</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="18">
         <v>83.6</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="18">
         <v>24.8</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="18">
         <v>95.6</v>
       </c>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="17">
         <v>2010</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="18">
         <v>15.8</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="18">
         <v>89.5</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="18">
         <v>8</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="18">
         <v>79.3</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="18">
         <v>18.8</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="18">
         <v>92.9</v>
       </c>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="17">
         <v>2010</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="18">
         <v>23</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="18">
         <v>92.2</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="18">
         <v>12.2</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="18">
         <v>85.7</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="18">
         <v>27.7</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="18">
         <v>94.9</v>
       </c>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="17">
         <v>2011</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="18">
         <v>18.600000000000001</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="18">
         <v>91.6</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="18">
         <v>9.2360000000000007</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="18">
         <v>82.67</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="18">
         <v>22.46</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="18">
         <v>94.668999999999997</v>
       </c>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="17">
         <v>2011</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="18">
         <v>25.2</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="18">
         <v>93</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="18">
         <v>13.965999999999999</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="18">
         <v>84.924000000000007</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="18">
         <v>30.058</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="18">
         <v>96.557000000000002</v>
       </c>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="17">
         <v>2012</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="18">
         <v>22.1</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="18">
         <v>92.6</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="20">
         <v>12</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="20">
         <v>79</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="20">
         <v>26</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="20">
         <v>98</v>
       </c>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="17">
         <v>2012</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="18">
         <v>27.6</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="18">
         <v>93.4</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="20">
         <v>16</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="20">
         <v>87</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="20">
         <v>33</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="20">
         <v>96</v>
       </c>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="17">
         <v>2013</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="18">
         <v>24.4</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="18">
         <v>93.6</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="20">
         <v>13</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="20">
         <v>74</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="20">
         <v>29</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="20">
         <v>102</v>
       </c>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="17">
         <v>2013</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="18">
         <v>29.3</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="18">
         <v>93.6</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="20">
         <v>17</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="20">
         <v>85</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="20">
         <v>35</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="20">
         <v>98</v>
       </c>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="17">
         <v>2014</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="18">
         <v>27.9</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="18">
         <v>93.7</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="20">
         <v>15</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="20">
         <v>72</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="20">
         <v>33</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="20">
         <v>103</v>
       </c>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="17">
         <v>2014</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="18">
         <v>32.299999999999997</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="18">
         <v>93.6</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="20">
         <v>20</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="20">
         <v>85</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="20">
         <v>38</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="20">
         <v>98</v>
       </c>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="17">
         <v>2015</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="18">
         <v>28.3</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="18">
         <v>94.8</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="20">
         <v>15</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="20">
         <v>77</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="20">
         <v>34</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="21">
         <v>102</v>
       </c>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="17">
         <v>2015</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="18">
         <v>32.9</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="18">
         <v>94.9</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="20">
         <v>22</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="20">
         <v>90</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="20">
         <v>38</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="21">
         <v>97</v>
       </c>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="17">
         <v>2016</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="22">
         <v>28.4</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="22">
         <v>93.2</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="20">
         <v>15</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="20">
         <v>78</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="20">
         <v>34</v>
       </c>
-      <c r="I25" s="29">
+      <c r="I25" s="20">
         <v>100</v>
       </c>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="17">
         <v>2016</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="18">
         <v>32.700000000000003</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="18">
         <v>93.6</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="20">
         <v>21</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="20">
         <v>88</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="20">
         <v>38</v>
       </c>
-      <c r="I26" s="29">
+      <c r="I26" s="20">
         <v>96</v>
       </c>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="17">
         <v>2017</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="22">
         <v>29.6</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="22">
         <v>93.2</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="20">
         <v>15</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="20">
         <v>71</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="20">
         <v>37</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="22">
         <v>104</v>
       </c>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="17">
         <v>2017</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="18">
         <v>33.1</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="18">
         <v>93.4</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="20">
         <v>20</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="20">
         <v>84</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="20">
         <v>40</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I28" s="21">
         <v>98</v>
       </c>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="17">
         <v>2018</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="18">
         <v>30.9</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="18">
         <v>92.8</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="22">
         <v>15</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="22">
         <v>73</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H29" s="22">
         <v>39</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="22">
         <v>103</v>
       </c>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="17">
         <v>2018</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="18">
         <v>33.6</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="18">
         <v>93</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="20">
         <v>20</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30" s="20">
         <v>82</v>
       </c>
-      <c r="H30" s="29">
-        <v>60</v>
-      </c>
-      <c r="I30" s="30">
+      <c r="H30" s="20">
+        <v>41</v>
+      </c>
+      <c r="I30" s="21">
         <v>100</v>
       </c>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="26" t="s">
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="17">
         <v>2019</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="18">
         <v>32.1</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="18">
         <v>92.7</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="20">
         <v>16</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="20">
         <v>78</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="20">
         <v>41</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="20">
         <v>100</v>
       </c>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="26" t="s">
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="17">
         <v>2019</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="18">
         <v>34.299999999999997</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="18">
         <v>93</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="20">
         <v>21</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="20">
         <v>81</v>
       </c>
-      <c r="H32" s="29">
+      <c r="H32" s="20">
         <v>42</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="20">
         <v>100</v>
       </c>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="26" t="s">
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="11">
         <v>2020</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="18">
         <v>32.9</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="18">
         <v>92.2</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="20">
         <v>17</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="20">
         <v>75</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="20">
         <v>42</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="20">
         <v>101</v>
       </c>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="34" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="26" t="s">
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="11">
         <v>2020</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="18">
         <v>35</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="18">
         <v>92.5</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="20">
         <v>21</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="20">
         <v>81</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="20">
         <v>43</v>
       </c>
-      <c r="I34" s="29">
+      <c r="I34" s="20">
         <v>99</v>
       </c>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="2:10" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="26" t="s">
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="2:10" s="23" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="11">
         <v>2021</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="20">
         <v>31.9</v>
       </c>
-      <c r="E35" s="29">
+      <c r="E35" s="20">
         <v>91.6</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="2:10" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="26" t="s">
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="2:10" s="23" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="11">
         <v>2021</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="20">
         <v>34.4</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E36" s="20">
         <v>91.9</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="20"/>
-    </row>
-    <row r="37" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="26"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="24"/>
-    </row>
-    <row r="38" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="24"/>
-    </row>
-    <row r="39" spans="2:10" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="17"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="27"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="2:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="20"/>
-    </row>
-    <row r="40" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-    </row>
-    <row r="41" spans="2:10" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="2:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="21"/>
-    </row>
-    <row r="42" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="22" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="22" t="s">
+    <row r="44" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="22" t="s">
+    <row r="45" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
+    <row r="46" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="2:10" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:10" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B41:I41"/>

</xml_diff>